<commit_message>
new info in seguridad informatica para equipos tecnicos
</commit_message>
<xml_diff>
--- a/5 Curso de Redes de Internet Profesional/3-mascaras-ejemplo_9e631794-660a-4d72-8a38-c75d33c38b6b.xlsx
+++ b/5 Curso de Redes de Internet Profesional/3-mascaras-ejemplo_9e631794-660a-4d72-8a38-c75d33c38b6b.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28025"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\courses\Platzi\2 Especialista en Ciberseguridad\4 Curso de Redes Informaticas de Internet\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B00DD3A-2ED8-49F4-B747-997C6D97A475}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="13940" tabRatio="500"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -52,7 +58,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -304,7 +310,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -330,18 +336,6 @@
     </xf>
     <xf numFmtId="1" fontId="2" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -370,26 +364,44 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="13">
-    <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -714,261 +726,261 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AF11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="180" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10:M11"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="180" workbookViewId="0">
+      <selection activeCell="T8" sqref="T8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="8" width="3.33203125" style="1" customWidth="1"/>
-    <col min="9" max="16" width="3.33203125" style="2" customWidth="1"/>
-    <col min="17" max="24" width="3.33203125" style="4" customWidth="1"/>
-    <col min="25" max="32" width="3.33203125" style="3" customWidth="1"/>
-    <col min="33" max="290" width="4.83203125" customWidth="1"/>
+    <col min="1" max="8" width="3.375" style="1" customWidth="1"/>
+    <col min="9" max="16" width="3.375" style="2" customWidth="1"/>
+    <col min="17" max="24" width="3.375" style="4" customWidth="1"/>
+    <col min="25" max="32" width="3.375" style="3" customWidth="1"/>
+    <col min="33" max="290" width="4.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32">
-      <c r="A1" s="17">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A1" s="13">
         <v>31</v>
       </c>
-      <c r="B1" s="18">
+      <c r="B1" s="14">
         <v>30</v>
       </c>
-      <c r="C1" s="18">
+      <c r="C1" s="14">
         <v>29</v>
       </c>
-      <c r="D1" s="18">
+      <c r="D1" s="14">
         <v>28</v>
       </c>
-      <c r="E1" s="18">
+      <c r="E1" s="14">
         <v>27</v>
       </c>
-      <c r="F1" s="18">
+      <c r="F1" s="14">
         <v>26</v>
       </c>
-      <c r="G1" s="18">
+      <c r="G1" s="14">
         <v>25</v>
       </c>
-      <c r="H1" s="18">
+      <c r="H1" s="14">
         <v>24</v>
       </c>
-      <c r="I1" s="19">
+      <c r="I1" s="15">
         <v>23</v>
       </c>
-      <c r="J1" s="19">
+      <c r="J1" s="15">
         <v>22</v>
       </c>
-      <c r="K1" s="19">
+      <c r="K1" s="15">
         <v>21</v>
       </c>
-      <c r="L1" s="19">
+      <c r="L1" s="15">
         <v>20</v>
       </c>
-      <c r="M1" s="19">
+      <c r="M1" s="15">
         <v>19</v>
       </c>
-      <c r="N1" s="19">
+      <c r="N1" s="15">
         <v>18</v>
       </c>
-      <c r="O1" s="19">
+      <c r="O1" s="15">
         <v>17</v>
       </c>
-      <c r="P1" s="19">
+      <c r="P1" s="15">
         <v>16</v>
       </c>
-      <c r="Q1" s="20">
+      <c r="Q1" s="16">
         <v>15</v>
       </c>
-      <c r="R1" s="20">
+      <c r="R1" s="16">
         <v>14</v>
       </c>
-      <c r="S1" s="20">
+      <c r="S1" s="16">
         <v>13</v>
       </c>
-      <c r="T1" s="20">
+      <c r="T1" s="16">
         <v>12</v>
       </c>
-      <c r="U1" s="20">
+      <c r="U1" s="16">
         <v>11</v>
       </c>
-      <c r="V1" s="20">
+      <c r="V1" s="16">
         <v>10</v>
       </c>
-      <c r="W1" s="20">
+      <c r="W1" s="16">
         <v>9</v>
       </c>
-      <c r="X1" s="20">
+      <c r="X1" s="16">
         <v>8</v>
       </c>
-      <c r="Y1" s="21">
+      <c r="Y1" s="17">
         <v>7</v>
       </c>
-      <c r="Z1" s="21">
+      <c r="Z1" s="17">
         <v>6</v>
       </c>
-      <c r="AA1" s="21">
+      <c r="AA1" s="17">
         <v>5</v>
       </c>
-      <c r="AB1" s="21">
+      <c r="AB1" s="17">
         <v>4</v>
       </c>
-      <c r="AC1" s="21">
+      <c r="AC1" s="17">
         <v>3</v>
       </c>
-      <c r="AD1" s="21">
-        <v>2</v>
-      </c>
-      <c r="AE1" s="21">
-        <v>1</v>
-      </c>
-      <c r="AF1" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:32" ht="16" thickBot="1">
-      <c r="A2" s="23">
-        <v>2</v>
-      </c>
-      <c r="B2" s="24">
-        <v>2</v>
-      </c>
-      <c r="C2" s="24">
-        <v>2</v>
-      </c>
-      <c r="D2" s="24">
-        <v>2</v>
-      </c>
-      <c r="E2" s="24">
-        <v>2</v>
-      </c>
-      <c r="F2" s="24">
-        <v>2</v>
-      </c>
-      <c r="G2" s="24">
-        <v>2</v>
-      </c>
-      <c r="H2" s="24">
-        <v>2</v>
-      </c>
-      <c r="I2" s="25">
-        <v>2</v>
-      </c>
-      <c r="J2" s="25">
-        <v>2</v>
-      </c>
-      <c r="K2" s="25">
-        <v>2</v>
-      </c>
-      <c r="L2" s="25">
-        <v>2</v>
-      </c>
-      <c r="M2" s="25">
-        <v>2</v>
-      </c>
-      <c r="N2" s="25">
-        <v>2</v>
-      </c>
-      <c r="O2" s="25">
-        <v>2</v>
-      </c>
-      <c r="P2" s="25">
-        <v>2</v>
-      </c>
-      <c r="Q2" s="26">
-        <v>2</v>
-      </c>
-      <c r="R2" s="26">
-        <v>2</v>
-      </c>
-      <c r="S2" s="26">
-        <v>2</v>
-      </c>
-      <c r="T2" s="26">
-        <v>2</v>
-      </c>
-      <c r="U2" s="26">
-        <v>2</v>
-      </c>
-      <c r="V2" s="26">
-        <v>2</v>
-      </c>
-      <c r="W2" s="26">
-        <v>2</v>
-      </c>
-      <c r="X2" s="26">
-        <v>2</v>
-      </c>
-      <c r="Y2" s="27">
-        <v>2</v>
-      </c>
-      <c r="Z2" s="27">
-        <v>2</v>
-      </c>
-      <c r="AA2" s="27">
-        <v>2</v>
-      </c>
-      <c r="AB2" s="27">
-        <v>2</v>
-      </c>
-      <c r="AC2" s="27">
-        <v>2</v>
-      </c>
-      <c r="AD2" s="27">
-        <v>2</v>
-      </c>
-      <c r="AE2" s="27">
-        <v>2</v>
-      </c>
-      <c r="AF2" s="28">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:32">
-      <c r="A3" s="12">
+      <c r="AD1" s="17">
+        <v>2</v>
+      </c>
+      <c r="AE1" s="17">
+        <v>1</v>
+      </c>
+      <c r="AF1" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:32" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="19">
+        <v>2</v>
+      </c>
+      <c r="B2" s="20">
+        <v>2</v>
+      </c>
+      <c r="C2" s="20">
+        <v>2</v>
+      </c>
+      <c r="D2" s="20">
+        <v>2</v>
+      </c>
+      <c r="E2" s="20">
+        <v>2</v>
+      </c>
+      <c r="F2" s="20">
+        <v>2</v>
+      </c>
+      <c r="G2" s="20">
+        <v>2</v>
+      </c>
+      <c r="H2" s="20">
+        <v>2</v>
+      </c>
+      <c r="I2" s="21">
+        <v>2</v>
+      </c>
+      <c r="J2" s="21">
+        <v>2</v>
+      </c>
+      <c r="K2" s="21">
+        <v>2</v>
+      </c>
+      <c r="L2" s="21">
+        <v>2</v>
+      </c>
+      <c r="M2" s="21">
+        <v>2</v>
+      </c>
+      <c r="N2" s="21">
+        <v>2</v>
+      </c>
+      <c r="O2" s="21">
+        <v>2</v>
+      </c>
+      <c r="P2" s="21">
+        <v>2</v>
+      </c>
+      <c r="Q2" s="22">
+        <v>2</v>
+      </c>
+      <c r="R2" s="22">
+        <v>2</v>
+      </c>
+      <c r="S2" s="22">
+        <v>2</v>
+      </c>
+      <c r="T2" s="22">
+        <v>2</v>
+      </c>
+      <c r="U2" s="22">
+        <v>2</v>
+      </c>
+      <c r="V2" s="22">
+        <v>2</v>
+      </c>
+      <c r="W2" s="22">
+        <v>2</v>
+      </c>
+      <c r="X2" s="22">
+        <v>2</v>
+      </c>
+      <c r="Y2" s="23">
+        <v>2</v>
+      </c>
+      <c r="Z2" s="23">
+        <v>2</v>
+      </c>
+      <c r="AA2" s="23">
+        <v>2</v>
+      </c>
+      <c r="AB2" s="23">
+        <v>2</v>
+      </c>
+      <c r="AC2" s="23">
+        <v>2</v>
+      </c>
+      <c r="AD2" s="23">
+        <v>2</v>
+      </c>
+      <c r="AE2" s="23">
+        <v>2</v>
+      </c>
+      <c r="AF2" s="24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A3" s="25">
         <v>255</v>
       </c>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="13">
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="26">
         <v>255</v>
       </c>
-      <c r="J3" s="13"/>
-      <c r="K3" s="13"/>
-      <c r="L3" s="13"/>
-      <c r="M3" s="13"/>
-      <c r="N3" s="13"/>
-      <c r="O3" s="13"/>
-      <c r="P3" s="13"/>
-      <c r="Q3" s="14">
+      <c r="J3" s="26"/>
+      <c r="K3" s="26"/>
+      <c r="L3" s="26"/>
+      <c r="M3" s="26"/>
+      <c r="N3" s="26"/>
+      <c r="O3" s="26"/>
+      <c r="P3" s="26"/>
+      <c r="Q3" s="27">
         <v>128</v>
       </c>
-      <c r="R3" s="14"/>
-      <c r="S3" s="14"/>
-      <c r="T3" s="14"/>
-      <c r="U3" s="14"/>
-      <c r="V3" s="14"/>
-      <c r="W3" s="14"/>
-      <c r="X3" s="14"/>
-      <c r="Y3" s="15">
-        <v>0</v>
-      </c>
-      <c r="Z3" s="15"/>
-      <c r="AA3" s="15"/>
-      <c r="AB3" s="15"/>
-      <c r="AC3" s="15"/>
-      <c r="AD3" s="15"/>
-      <c r="AE3" s="15"/>
-      <c r="AF3" s="15"/>
-    </row>
-    <row r="4" spans="1:32">
+      <c r="R3" s="27"/>
+      <c r="S3" s="27"/>
+      <c r="T3" s="27"/>
+      <c r="U3" s="27"/>
+      <c r="V3" s="27"/>
+      <c r="W3" s="27"/>
+      <c r="X3" s="27"/>
+      <c r="Y3" s="28">
+        <v>0</v>
+      </c>
+      <c r="Z3" s="28"/>
+      <c r="AA3" s="28"/>
+      <c r="AB3" s="28"/>
+      <c r="AC3" s="28"/>
+      <c r="AD3" s="28"/>
+      <c r="AE3" s="28"/>
+      <c r="AF3" s="28"/>
+    </row>
+    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -1066,95 +1078,95 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:32">
-      <c r="A5" s="12">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A5" s="25">
         <v>255</v>
       </c>
-      <c r="B5" s="12"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="13">
+      <c r="B5" s="25"/>
+      <c r="C5" s="25"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="25"/>
+      <c r="G5" s="25"/>
+      <c r="H5" s="25"/>
+      <c r="I5" s="26">
         <v>240</v>
       </c>
-      <c r="J5" s="13"/>
-      <c r="K5" s="13"/>
-      <c r="L5" s="13"/>
-      <c r="M5" s="13"/>
-      <c r="N5" s="13"/>
-      <c r="O5" s="13"/>
-      <c r="P5" s="13"/>
-      <c r="Q5" s="14">
-        <v>0</v>
-      </c>
-      <c r="R5" s="14"/>
-      <c r="S5" s="14"/>
-      <c r="T5" s="14"/>
-      <c r="U5" s="14"/>
-      <c r="V5" s="14"/>
-      <c r="W5" s="14"/>
-      <c r="X5" s="14"/>
-      <c r="Y5" s="15">
-        <v>0</v>
-      </c>
-      <c r="Z5" s="15"/>
-      <c r="AA5" s="15"/>
-      <c r="AB5" s="15"/>
-      <c r="AC5" s="15"/>
-      <c r="AD5" s="15"/>
-      <c r="AE5" s="15"/>
-      <c r="AF5" s="15"/>
-    </row>
-    <row r="6" spans="1:32">
-      <c r="A6" s="29">
-        <v>1</v>
-      </c>
-      <c r="B6" s="29">
-        <v>1</v>
-      </c>
-      <c r="C6" s="29">
-        <v>1</v>
-      </c>
-      <c r="D6" s="29">
-        <v>1</v>
-      </c>
-      <c r="E6" s="29">
-        <v>1</v>
-      </c>
-      <c r="F6" s="29">
-        <v>1</v>
-      </c>
-      <c r="G6" s="29">
-        <v>1</v>
-      </c>
-      <c r="H6" s="29">
-        <v>1</v>
-      </c>
-      <c r="I6" s="30">
-        <v>1</v>
-      </c>
-      <c r="J6" s="30">
-        <v>1</v>
-      </c>
-      <c r="K6" s="30">
-        <v>1</v>
-      </c>
-      <c r="L6" s="30">
-        <v>1</v>
-      </c>
-      <c r="M6" s="30">
-        <v>0</v>
-      </c>
-      <c r="N6" s="30">
-        <v>0</v>
-      </c>
-      <c r="O6" s="30">
-        <v>0</v>
-      </c>
-      <c r="P6" s="30">
+      <c r="J5" s="26"/>
+      <c r="K5" s="26"/>
+      <c r="L5" s="26"/>
+      <c r="M5" s="26"/>
+      <c r="N5" s="26"/>
+      <c r="O5" s="26"/>
+      <c r="P5" s="26"/>
+      <c r="Q5" s="27">
+        <v>0</v>
+      </c>
+      <c r="R5" s="27"/>
+      <c r="S5" s="27"/>
+      <c r="T5" s="27"/>
+      <c r="U5" s="27"/>
+      <c r="V5" s="27"/>
+      <c r="W5" s="27"/>
+      <c r="X5" s="27"/>
+      <c r="Y5" s="28">
+        <v>0</v>
+      </c>
+      <c r="Z5" s="28"/>
+      <c r="AA5" s="28"/>
+      <c r="AB5" s="28"/>
+      <c r="AC5" s="28"/>
+      <c r="AD5" s="28"/>
+      <c r="AE5" s="28"/>
+      <c r="AF5" s="28"/>
+    </row>
+    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>1</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1</v>
+      </c>
+      <c r="D6" s="1">
+        <v>1</v>
+      </c>
+      <c r="E6" s="1">
+        <v>1</v>
+      </c>
+      <c r="F6" s="1">
+        <v>1</v>
+      </c>
+      <c r="G6" s="1">
+        <v>1</v>
+      </c>
+      <c r="H6" s="1">
+        <v>1</v>
+      </c>
+      <c r="I6" s="2">
+        <v>1</v>
+      </c>
+      <c r="J6" s="2">
+        <v>1</v>
+      </c>
+      <c r="K6" s="2">
+        <v>1</v>
+      </c>
+      <c r="L6" s="2">
+        <v>1</v>
+      </c>
+      <c r="M6" s="2">
+        <v>0</v>
+      </c>
+      <c r="N6" s="2">
+        <v>0</v>
+      </c>
+      <c r="O6" s="2">
+        <v>0</v>
+      </c>
+      <c r="P6" s="2">
         <v>0</v>
       </c>
       <c r="Q6" s="4">
@@ -1206,60 +1218,148 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:32">
-      <c r="A7" s="12"/>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="13"/>
-      <c r="J7" s="13"/>
-      <c r="K7" s="13"/>
-      <c r="L7" s="13"/>
-      <c r="M7" s="13"/>
-      <c r="N7" s="13"/>
-      <c r="O7" s="13"/>
-      <c r="P7" s="13"/>
-      <c r="Q7" s="14"/>
-      <c r="R7" s="14"/>
-      <c r="S7" s="14"/>
-      <c r="T7" s="14"/>
-      <c r="U7" s="14"/>
-      <c r="V7" s="14"/>
-      <c r="W7" s="14"/>
-      <c r="X7" s="14"/>
-      <c r="Y7" s="15"/>
-      <c r="Z7" s="15"/>
-      <c r="AA7" s="15"/>
-      <c r="AB7" s="15"/>
-      <c r="AC7" s="15"/>
-      <c r="AD7" s="15"/>
-      <c r="AE7" s="15"/>
-      <c r="AF7" s="15"/>
-    </row>
-    <row r="8" spans="1:32">
-      <c r="A8" s="29"/>
-      <c r="B8" s="29"/>
-      <c r="C8" s="29"/>
-      <c r="D8" s="29"/>
-      <c r="E8" s="29"/>
-      <c r="F8" s="29"/>
-      <c r="G8" s="29"/>
-      <c r="H8" s="29"/>
-      <c r="I8" s="30"/>
-      <c r="J8" s="30"/>
-      <c r="K8" s="30"/>
-      <c r="L8" s="30"/>
-      <c r="M8" s="30"/>
-      <c r="N8" s="30"/>
-      <c r="O8" s="30"/>
-      <c r="P8" s="30"/>
-    </row>
-    <row r="11" spans="1:32">
-      <c r="M11" s="16"/>
+    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A7" s="25">
+        <v>255</v>
+      </c>
+      <c r="B7" s="25"/>
+      <c r="C7" s="25"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="25"/>
+      <c r="H7" s="25"/>
+      <c r="I7" s="26">
+        <v>255</v>
+      </c>
+      <c r="J7" s="26"/>
+      <c r="K7" s="26"/>
+      <c r="L7" s="26"/>
+      <c r="M7" s="26"/>
+      <c r="N7" s="26"/>
+      <c r="O7" s="26"/>
+      <c r="P7" s="26"/>
+      <c r="Q7" s="27">
+        <v>224</v>
+      </c>
+      <c r="R7" s="27"/>
+      <c r="S7" s="27"/>
+      <c r="T7" s="27"/>
+      <c r="U7" s="27"/>
+      <c r="V7" s="27"/>
+      <c r="W7" s="27"/>
+      <c r="X7" s="27"/>
+      <c r="Y7" s="28">
+        <v>0</v>
+      </c>
+      <c r="Z7" s="28"/>
+      <c r="AA7" s="28"/>
+      <c r="AB7" s="28"/>
+      <c r="AC7" s="28"/>
+      <c r="AD7" s="28"/>
+      <c r="AE7" s="28"/>
+      <c r="AF7" s="28"/>
+    </row>
+    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>1</v>
+      </c>
+      <c r="B8" s="1">
+        <v>1</v>
+      </c>
+      <c r="C8" s="1">
+        <v>1</v>
+      </c>
+      <c r="D8" s="1">
+        <v>1</v>
+      </c>
+      <c r="E8" s="1">
+        <v>1</v>
+      </c>
+      <c r="F8" s="1">
+        <v>1</v>
+      </c>
+      <c r="G8" s="1">
+        <v>1</v>
+      </c>
+      <c r="H8" s="1">
+        <v>1</v>
+      </c>
+      <c r="I8" s="2">
+        <v>1</v>
+      </c>
+      <c r="J8" s="2">
+        <v>1</v>
+      </c>
+      <c r="K8" s="2">
+        <v>1</v>
+      </c>
+      <c r="L8" s="2">
+        <v>1</v>
+      </c>
+      <c r="M8" s="2">
+        <v>1</v>
+      </c>
+      <c r="N8" s="2">
+        <v>1</v>
+      </c>
+      <c r="O8" s="2">
+        <v>1</v>
+      </c>
+      <c r="P8" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q8" s="4">
+        <v>1</v>
+      </c>
+      <c r="R8" s="4">
+        <v>1</v>
+      </c>
+      <c r="S8" s="4">
+        <v>1</v>
+      </c>
+      <c r="T8" s="4">
+        <v>0</v>
+      </c>
+      <c r="U8" s="4">
+        <v>0</v>
+      </c>
+      <c r="V8" s="4">
+        <v>0</v>
+      </c>
+      <c r="W8" s="4">
+        <v>0</v>
+      </c>
+      <c r="X8" s="4">
+        <v>0</v>
+      </c>
+      <c r="Y8" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z8" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA8" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB8" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC8" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD8" s="3">
+        <v>0</v>
+      </c>
+      <c r="AE8" s="3">
+        <v>0</v>
+      </c>
+      <c r="AF8" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="M11" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -1287,19 +1387,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView topLeftCell="A2" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
       <selection activeCell="A7" sqref="A7:D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="9" max="9" width="34" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="28">
+    <row r="1" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>1</v>
       </c>
@@ -1328,7 +1428,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="28">
+    <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
         <v>128</v>
       </c>
@@ -1355,7 +1455,7 @@
       </c>
       <c r="I2" s="7"/>
     </row>
-    <row r="3" spans="1:9" ht="28">
+    <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
         <v>0</v>
       </c>
@@ -1384,7 +1484,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="28">
+    <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="9">
         <v>1</v>
       </c>
@@ -1413,7 +1513,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="28">
+    <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
         <v>1</v>
       </c>
@@ -1442,7 +1542,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="28">
+    <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="9">
         <v>1</v>
       </c>
@@ -1471,7 +1571,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="28">
+    <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
         <v>1</v>
       </c>
@@ -1500,7 +1600,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="28">
+    <row r="8" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="9">
         <v>1</v>
       </c>
@@ -1529,7 +1629,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="28">
+    <row r="9" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
         <v>1</v>
       </c>
@@ -1558,7 +1658,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="28">
+    <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
         <v>1</v>
       </c>
@@ -1587,7 +1687,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="28">
+    <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
         <v>1</v>
       </c>

</xml_diff>